<commit_message>
add 'type of storage'
</commit_message>
<xml_diff>
--- a/cmip6/machines/cmip6_ec-earth-consortium_machines.xlsx
+++ b/cmip6/machines/cmip6_ec-earth-consortium_machines.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2344" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2345" uniqueCount="334">
   <si>
     <t xml:space="preserve">ES-DOC CMIP6 Institute Machines</t>
   </si>
@@ -943,6 +943,9 @@
     <t xml:space="preserve">IBM General Parallel File System</t>
   </si>
   <si>
+    <t xml:space="preserve">GPFS: IBM GPFS (also known as IBM Spectral Scale.</t>
+  </si>
+  <si>
     <t xml:space="preserve">EC-Earth3</t>
   </si>
   <si>
@@ -11165,8 +11168,8 @@
   </sheetPr>
   <dimension ref="A1:F869"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B368" activeCellId="0" sqref="B368"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A277" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B303" activeCellId="0" sqref="B303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13530,7 +13533,9 @@
     </row>
     <row r="303" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A303" s="62"/>
-      <c r="B303" s="32"/>
+      <c r="B303" s="32" t="s">
+        <v>303</v>
+      </c>
       <c r="C303" s="32"/>
       <c r="D303" s="32"/>
     </row>
@@ -14089,7 +14094,7 @@
         <v>231</v>
       </c>
       <c r="B389" s="24" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C389" s="24"/>
       <c r="D389" s="24"/>
@@ -14112,7 +14117,7 @@
         <v>233</v>
       </c>
       <c r="B392" s="24" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C392" s="24"/>
       <c r="D392" s="24"/>
@@ -14135,7 +14140,7 @@
         <v>235</v>
       </c>
       <c r="B395" s="24" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C395" s="24"/>
       <c r="D395" s="24"/>
@@ -14158,7 +14163,7 @@
         <v>237</v>
       </c>
       <c r="B398" s="24" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C398" s="24"/>
       <c r="D398" s="24"/>
@@ -14181,7 +14186,7 @@
         <v>239</v>
       </c>
       <c r="B401" s="24" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C401" s="24"/>
       <c r="D401" s="24"/>
@@ -14204,7 +14209,7 @@
         <v>241</v>
       </c>
       <c r="B404" s="24" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C404" s="24"/>
       <c r="D404" s="24"/>
@@ -14224,10 +14229,10 @@
     </row>
     <row r="407" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A407" s="23" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B407" s="24" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C407" s="24"/>
       <c r="D407" s="24"/>
@@ -14247,10 +14252,10 @@
     </row>
     <row r="410" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A410" s="23" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B410" s="24" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C410" s="24"/>
       <c r="D410" s="24"/>
@@ -14270,10 +14275,10 @@
     </row>
     <row r="413" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A413" s="23" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B413" s="24" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C413" s="24"/>
       <c r="D413" s="24"/>
@@ -14293,10 +14298,10 @@
     </row>
     <row r="416" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A416" s="23" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B416" s="24" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C416" s="24"/>
       <c r="D416" s="24"/>
@@ -14316,10 +14321,10 @@
     </row>
     <row r="419" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A419" s="23" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B419" s="24" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C419" s="24"/>
       <c r="D419" s="24"/>
@@ -14485,7 +14490,7 @@
         <v>256</v>
       </c>
       <c r="B441" s="24" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C441" s="24"/>
       <c r="D441" s="24"/>
@@ -14577,7 +14582,7 @@
         <v>269</v>
       </c>
       <c r="B453" s="24" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C453" s="24"/>
       <c r="D453" s="24"/>
@@ -14827,7 +14832,7 @@
     </row>
     <row r="486" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B486" s="76" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C486" s="76"/>
       <c r="D486" s="76"/>
@@ -17552,7 +17557,7 @@
   </sheetPr>
   <dimension ref="A1:F869"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A349" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A277" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B368" activeCellId="0" sqref="B368"/>
     </sheetView>
   </sheetViews>
@@ -17644,7 +17649,7 @@
     </row>
     <row r="11" s="2" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="27" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C11" s="27"/>
       <c r="D11" s="27"/>
@@ -17792,7 +17797,7 @@
     </row>
     <row r="31" s="2" customFormat="true" ht="148.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="32" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C31" s="32"/>
       <c r="D31" s="32"/>
@@ -17831,7 +17836,7 @@
     </row>
     <row r="37" s="2" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="27" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C37" s="27"/>
       <c r="D37" s="27"/>
@@ -17995,7 +18000,7 @@
     </row>
     <row r="62" s="2" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="27" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C62" s="27"/>
       <c r="D62" s="27"/>
@@ -18789,7 +18794,7 @@
     </row>
     <row r="162" s="2" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="52" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F162" s="28"/>
     </row>
@@ -20472,7 +20477,7 @@
         <v>231</v>
       </c>
       <c r="B389" s="24" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C389" s="24"/>
       <c r="D389" s="24"/>
@@ -20495,7 +20500,7 @@
         <v>233</v>
       </c>
       <c r="B392" s="24" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C392" s="24"/>
       <c r="D392" s="24"/>
@@ -20518,7 +20523,7 @@
         <v>235</v>
       </c>
       <c r="B395" s="24" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C395" s="24"/>
       <c r="D395" s="24"/>
@@ -20541,7 +20546,7 @@
         <v>237</v>
       </c>
       <c r="B398" s="24" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C398" s="24"/>
       <c r="D398" s="24"/>
@@ -20564,7 +20569,7 @@
         <v>239</v>
       </c>
       <c r="B401" s="24" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C401" s="24"/>
       <c r="D401" s="24"/>
@@ -20587,7 +20592,7 @@
         <v>241</v>
       </c>
       <c r="B404" s="24" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C404" s="24"/>
       <c r="D404" s="24"/>
@@ -20607,10 +20612,10 @@
     </row>
     <row r="407" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A407" s="23" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B407" s="24" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C407" s="24"/>
       <c r="D407" s="24"/>
@@ -20630,10 +20635,10 @@
     </row>
     <row r="410" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A410" s="23" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B410" s="24" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C410" s="24"/>
       <c r="D410" s="24"/>
@@ -20653,10 +20658,10 @@
     </row>
     <row r="413" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A413" s="23" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B413" s="24" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C413" s="24"/>
       <c r="D413" s="24"/>
@@ -20676,10 +20681,10 @@
     </row>
     <row r="416" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A416" s="23" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B416" s="24" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C416" s="24"/>
       <c r="D416" s="24"/>
@@ -20699,10 +20704,10 @@
     </row>
     <row r="419" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A419" s="23" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B419" s="24" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C419" s="24"/>
       <c r="D419" s="24"/>
@@ -20868,7 +20873,7 @@
         <v>256</v>
       </c>
       <c r="B441" s="24" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C441" s="24"/>
       <c r="D441" s="24"/>
@@ -20960,7 +20965,7 @@
         <v>269</v>
       </c>
       <c r="B453" s="24" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C453" s="24"/>
       <c r="D453" s="24"/>
@@ -21210,7 +21215,7 @@
     </row>
     <row r="486" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B486" s="76" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C486" s="76"/>
       <c r="D486" s="76"/>
@@ -23935,7 +23940,7 @@
   </sheetPr>
   <dimension ref="A1:F869"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A352" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A277" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B374" activeCellId="0" sqref="B374"/>
     </sheetView>
   </sheetViews>
@@ -24027,7 +24032,7 @@
     </row>
     <row r="11" s="2" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="27" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C11" s="27"/>
       <c r="D11" s="27"/>
@@ -24212,7 +24217,7 @@
     </row>
     <row r="37" s="2" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="27" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C37" s="27"/>
       <c r="D37" s="27"/>
@@ -24293,7 +24298,7 @@
     </row>
     <row r="49" s="2" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="27" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C49" s="27"/>
       <c r="D49" s="27"/>
@@ -25170,7 +25175,7 @@
     </row>
     <row r="162" s="2" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="52" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F162" s="28"/>
     </row>
@@ -26853,7 +26858,7 @@
         <v>231</v>
       </c>
       <c r="B389" s="24" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C389" s="24"/>
       <c r="D389" s="24"/>
@@ -26876,7 +26881,7 @@
         <v>233</v>
       </c>
       <c r="B392" s="24" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C392" s="24"/>
       <c r="D392" s="24"/>
@@ -26899,7 +26904,7 @@
         <v>235</v>
       </c>
       <c r="B395" s="24" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C395" s="24"/>
       <c r="D395" s="24"/>
@@ -26922,7 +26927,7 @@
         <v>237</v>
       </c>
       <c r="B398" s="24" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C398" s="24"/>
       <c r="D398" s="24"/>
@@ -26945,7 +26950,7 @@
         <v>239</v>
       </c>
       <c r="B401" s="24" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C401" s="24"/>
       <c r="D401" s="24"/>
@@ -26968,7 +26973,7 @@
         <v>241</v>
       </c>
       <c r="B404" s="24" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C404" s="24"/>
       <c r="D404" s="24"/>
@@ -26988,10 +26993,10 @@
     </row>
     <row r="407" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A407" s="23" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B407" s="24" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C407" s="24"/>
       <c r="D407" s="24"/>
@@ -27011,10 +27016,10 @@
     </row>
     <row r="410" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A410" s="23" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B410" s="24" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C410" s="24"/>
       <c r="D410" s="24"/>
@@ -27034,10 +27039,10 @@
     </row>
     <row r="413" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A413" s="23" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B413" s="24" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C413" s="24"/>
       <c r="D413" s="24"/>
@@ -27057,10 +27062,10 @@
     </row>
     <row r="416" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A416" s="23" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B416" s="24" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C416" s="24"/>
       <c r="D416" s="24"/>
@@ -27080,10 +27085,10 @@
     </row>
     <row r="419" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A419" s="23" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B419" s="24" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C419" s="24"/>
       <c r="D419" s="24"/>
@@ -27249,7 +27254,7 @@
         <v>256</v>
       </c>
       <c r="B441" s="24" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C441" s="24"/>
       <c r="D441" s="24"/>
@@ -27341,7 +27346,7 @@
         <v>269</v>
       </c>
       <c r="B453" s="24" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C453" s="24"/>
       <c r="D453" s="24"/>
@@ -27591,7 +27596,7 @@
     </row>
     <row r="486" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B486" s="76" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C486" s="76"/>
       <c r="D486" s="76"/>
@@ -30316,7 +30321,7 @@
   </sheetPr>
   <dimension ref="A1:F869"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A286" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B166" activeCellId="0" sqref="B166"/>
     </sheetView>
   </sheetViews>
@@ -30408,7 +30413,7 @@
     </row>
     <row r="11" s="2" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="27" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C11" s="27"/>
       <c r="D11" s="27"/>
@@ -30672,7 +30677,7 @@
     </row>
     <row r="49" s="2" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="27" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C49" s="27"/>
       <c r="D49" s="27"/>
@@ -31545,7 +31550,7 @@
     </row>
     <row r="162" s="2" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="52" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F162" s="28"/>
     </row>
@@ -33224,7 +33229,7 @@
         <v>231</v>
       </c>
       <c r="B389" s="24" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C389" s="24"/>
       <c r="D389" s="24"/>
@@ -33247,7 +33252,7 @@
         <v>233</v>
       </c>
       <c r="B392" s="24" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C392" s="24"/>
       <c r="D392" s="24"/>
@@ -33270,7 +33275,7 @@
         <v>235</v>
       </c>
       <c r="B395" s="24" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C395" s="24"/>
       <c r="D395" s="24"/>
@@ -33293,7 +33298,7 @@
         <v>237</v>
       </c>
       <c r="B398" s="24" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C398" s="24"/>
       <c r="D398" s="24"/>
@@ -33316,7 +33321,7 @@
         <v>239</v>
       </c>
       <c r="B401" s="24" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C401" s="24"/>
       <c r="D401" s="24"/>
@@ -33339,7 +33344,7 @@
         <v>241</v>
       </c>
       <c r="B404" s="24" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C404" s="24"/>
       <c r="D404" s="24"/>
@@ -33359,10 +33364,10 @@
     </row>
     <row r="407" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A407" s="23" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B407" s="24" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C407" s="24"/>
       <c r="D407" s="24"/>
@@ -33382,10 +33387,10 @@
     </row>
     <row r="410" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A410" s="23" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B410" s="24" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C410" s="24"/>
       <c r="D410" s="24"/>
@@ -33405,10 +33410,10 @@
     </row>
     <row r="413" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A413" s="23" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B413" s="24" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C413" s="24"/>
       <c r="D413" s="24"/>
@@ -33428,10 +33433,10 @@
     </row>
     <row r="416" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A416" s="23" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B416" s="24" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C416" s="24"/>
       <c r="D416" s="24"/>
@@ -33451,10 +33456,10 @@
     </row>
     <row r="419" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A419" s="23" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B419" s="24" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C419" s="24"/>
       <c r="D419" s="24"/>
@@ -33620,7 +33625,7 @@
         <v>256</v>
       </c>
       <c r="B441" s="24" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C441" s="24"/>
       <c r="D441" s="24"/>
@@ -33712,7 +33717,7 @@
         <v>269</v>
       </c>
       <c r="B453" s="24" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C453" s="24"/>
       <c r="D453" s="24"/>
@@ -33962,7 +33967,7 @@
     </row>
     <row r="486" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B486" s="76" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C486" s="76"/>
       <c r="D486" s="76"/>

</xml_diff>